<commit_message>
use ; to separate LandVoc concepts related
</commit_message>
<xml_diff>
--- a/landlibrary/examples/Land Library Metadata Example (Land Portal).xlsx
+++ b/landlibrary/examples/Land Library Metadata Example (Land Portal).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\data\landlibrary\importers\Simple Land Portal CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\data\landlibrary\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -40,6 +40,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Person author</t>
         </r>
@@ -52,6 +53,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>If there is no person author but only the organization is listed, this is a "corporate author".</t>
         </r>
@@ -64,6 +66,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Organization that published the resource originally (needs to have an organizational profile on LP)</t>
         </r>
@@ -77,6 +80,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>In case of a file upload, put a / and the name of the file.</t>
         </r>
@@ -99,6 +103,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Person author</t>
         </r>
@@ -111,6 +116,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>If there is no person author but only the organization is listed, this is a "corporate author".</t>
         </r>
@@ -123,6 +129,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Organization that published the resource originally (needs to have an organizational profile on LP)</t>
         </r>
@@ -136,6 +143,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Organization that owns the resource.</t>
         </r>
@@ -196,9 +204,6 @@
     <t>http://www.nature.com/articles/srep29987.pdf</t>
   </si>
   <si>
-    <t>agricultural land management, agroforestry systems, climate change, environment, forestry, sustainable land management, sustainable land use</t>
-  </si>
-  <si>
     <t>Land Use, Management &amp; Investment</t>
   </si>
   <si>
@@ -345,6 +350,9 @@
   </si>
   <si>
     <t>(ideally from a our list)</t>
+  </si>
+  <si>
+    <t>agricultural land management; agroforestry systems; climate change; environment; forestry; sustainable land management; sustainable land use</t>
   </si>
 </sst>
 </file>
@@ -363,12 +371,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -744,7 +754,7 @@
   <dimension ref="A1:V198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -787,13 +797,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>7</v>
@@ -814,19 +824,19 @@
         <v>12</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -837,52 +847,52 @@
         <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1">
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -890,28 +900,28 @@
     </row>
     <row r="3" spans="1:22" s="9" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="9">
         <v>35</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="10">
         <v>41656</v>
@@ -920,31 +930,31 @@
         <v>9</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="R3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1607,13 +1617,13 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>7</v>
@@ -1634,148 +1644,148 @@
         <v>12</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated example XLSX file
</commit_message>
<xml_diff>
--- a/landlibrary/examples/Land Library Metadata Example (Land Portal).xlsx
+++ b/landlibrary/examples/Land Library Metadata Example (Land Portal).xlsx
@@ -31,6 +31,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Lisette</author>
+    <author>carlos</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0">
@@ -69,6 +70,48 @@
             <family val="2"/>
           </rPr>
           <t>Organization that published the resource originally (needs to have an organizational profile on LP)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ideally ISO 639-1 code</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ideally, the ISO 3166-1 alpha-3 code for countries and UN M49 code for areas/regions</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the language of the metadata itself</t>
         </r>
       </text>
     </comment>
@@ -154,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>Abstract/Description</t>
   </si>
@@ -353,13 +396,19 @@
   </si>
   <si>
     <t>agricultural land management; agroforestry systems; climate change; environment; forestry; sustainable land management; sustainable land use</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>Metadata language</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -409,6 +458,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -431,17 +494,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -457,19 +511,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -754,811 +820,810 @@
   <dimension ref="A1:V198"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.8984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
-    <col min="6" max="7" width="16.09765625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.09765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.8984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.8984375" style="8" customWidth="1"/>
-    <col min="12" max="13" width="13.09765625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.8984375" customWidth="1"/>
-    <col min="16" max="16" width="22.69921875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5" style="3" customWidth="1"/>
-    <col min="18" max="18" width="20.296875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="27" style="1" customWidth="1"/>
-    <col min="20" max="22" width="10.8984375" style="3"/>
-    <col min="23" max="16384" width="10.8984375" style="1"/>
+    <col min="1" max="1" width="36.09765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.69921875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.09765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.69921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.8984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.69921875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="33.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="29.3984375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="24.59765625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.59765625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.19921875" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.8984375" style="13"/>
+    <col min="23" max="16384" width="10.8984375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="7" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:22" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="T1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="109.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:22" s="10" customFormat="1" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="10">
+        <v>35</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="11">
+        <v>41656</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-    </row>
-    <row r="3" spans="1:22" s="9" customFormat="1" ht="135.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="10">
-        <v>41656</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
+      <c r="T3" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O5" s="1"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O6" s="1"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O7" s="1"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O8" s="1"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O9" s="1"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O10" s="1"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O11" s="1"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O12" s="1"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O13" s="1"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O14" s="1"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O15" s="1"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="O16" s="1"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O17" s="1"/>
+      <c r="O17" s="5"/>
     </row>
     <row r="18" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O18" s="1"/>
+      <c r="O18" s="5"/>
     </row>
     <row r="19" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O19" s="1"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O20" s="1"/>
+      <c r="O20" s="5"/>
     </row>
     <row r="21" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O21" s="1"/>
+      <c r="O21" s="5"/>
     </row>
     <row r="22" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O22" s="1"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O23" s="1"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O24" s="1"/>
+      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O25" s="1"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O26" s="1"/>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O27" s="1"/>
+      <c r="O27" s="5"/>
     </row>
     <row r="28" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O28" s="1"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O29" s="1"/>
+      <c r="O29" s="5"/>
     </row>
     <row r="30" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O30" s="1"/>
+      <c r="O30" s="5"/>
     </row>
     <row r="31" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O31" s="1"/>
+      <c r="O31" s="5"/>
     </row>
     <row r="32" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O32" s="1"/>
+      <c r="O32" s="5"/>
     </row>
     <row r="33" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O33" s="1"/>
+      <c r="O33" s="5"/>
     </row>
     <row r="34" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O34" s="1"/>
+      <c r="O34" s="5"/>
     </row>
     <row r="35" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O35" s="1"/>
+      <c r="O35" s="5"/>
     </row>
     <row r="36" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O36" s="1"/>
+      <c r="O36" s="5"/>
     </row>
     <row r="37" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O37" s="1"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O38" s="1"/>
+      <c r="O38" s="5"/>
     </row>
     <row r="39" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O39" s="1"/>
+      <c r="O39" s="5"/>
     </row>
     <row r="40" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O40" s="1"/>
+      <c r="O40" s="5"/>
     </row>
     <row r="41" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O41" s="1"/>
+      <c r="O41" s="5"/>
     </row>
     <row r="42" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O42" s="1"/>
+      <c r="O42" s="5"/>
     </row>
     <row r="43" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O43" s="1"/>
+      <c r="O43" s="5"/>
     </row>
     <row r="44" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O44" s="1"/>
+      <c r="O44" s="5"/>
     </row>
     <row r="45" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O45" s="1"/>
+      <c r="O45" s="5"/>
     </row>
     <row r="46" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O46" s="1"/>
+      <c r="O46" s="5"/>
     </row>
     <row r="47" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O47" s="1"/>
+      <c r="O47" s="5"/>
     </row>
     <row r="48" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O48" s="1"/>
+      <c r="O48" s="5"/>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O49" s="1"/>
+      <c r="O49" s="5"/>
     </row>
     <row r="50" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O50" s="1"/>
+      <c r="O50" s="5"/>
     </row>
     <row r="51" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O51" s="1"/>
+      <c r="O51" s="5"/>
     </row>
     <row r="52" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O52" s="1"/>
+      <c r="O52" s="5"/>
     </row>
     <row r="53" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O53" s="1"/>
+      <c r="O53" s="5"/>
     </row>
     <row r="54" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O54" s="1"/>
+      <c r="O54" s="5"/>
     </row>
     <row r="55" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O55" s="1"/>
+      <c r="O55" s="5"/>
     </row>
     <row r="56" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O56" s="1"/>
+      <c r="O56" s="5"/>
     </row>
     <row r="57" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O57" s="1"/>
+      <c r="O57" s="5"/>
     </row>
     <row r="58" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O58" s="1"/>
+      <c r="O58" s="5"/>
     </row>
     <row r="59" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O59" s="1"/>
+      <c r="O59" s="5"/>
     </row>
     <row r="60" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O60" s="1"/>
+      <c r="O60" s="5"/>
     </row>
     <row r="61" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O61" s="1"/>
+      <c r="O61" s="5"/>
     </row>
     <row r="62" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O62" s="1"/>
+      <c r="O62" s="5"/>
     </row>
     <row r="63" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O63" s="1"/>
+      <c r="O63" s="5"/>
     </row>
     <row r="64" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O64" s="1"/>
+      <c r="O64" s="5"/>
     </row>
     <row r="65" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O65" s="1"/>
+      <c r="O65" s="5"/>
     </row>
     <row r="66" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O66" s="1"/>
+      <c r="O66" s="5"/>
     </row>
     <row r="67" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O67" s="1"/>
+      <c r="O67" s="5"/>
     </row>
     <row r="68" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O68" s="1"/>
+      <c r="O68" s="5"/>
     </row>
     <row r="69" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O69" s="1"/>
+      <c r="O69" s="5"/>
     </row>
     <row r="70" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O70" s="1"/>
+      <c r="O70" s="5"/>
     </row>
     <row r="71" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O71" s="1"/>
+      <c r="O71" s="5"/>
     </row>
     <row r="72" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O72" s="1"/>
+      <c r="O72" s="5"/>
     </row>
     <row r="73" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O73" s="1"/>
+      <c r="O73" s="5"/>
     </row>
     <row r="74" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O74" s="1"/>
+      <c r="O74" s="5"/>
     </row>
     <row r="75" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O75" s="1"/>
+      <c r="O75" s="5"/>
     </row>
     <row r="76" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O76" s="1"/>
+      <c r="O76" s="5"/>
     </row>
     <row r="77" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O77" s="1"/>
+      <c r="O77" s="5"/>
     </row>
     <row r="78" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O78" s="1"/>
+      <c r="O78" s="5"/>
     </row>
     <row r="79" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O79" s="1"/>
+      <c r="O79" s="5"/>
     </row>
     <row r="80" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O80" s="1"/>
+      <c r="O80" s="5"/>
     </row>
     <row r="81" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O81" s="1"/>
+      <c r="O81" s="5"/>
     </row>
     <row r="82" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O82" s="1"/>
+      <c r="O82" s="5"/>
     </row>
     <row r="83" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O83" s="1"/>
+      <c r="O83" s="5"/>
     </row>
     <row r="84" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O84" s="1"/>
+      <c r="O84" s="5"/>
     </row>
     <row r="85" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O85" s="1"/>
+      <c r="O85" s="5"/>
     </row>
     <row r="86" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O86" s="1"/>
+      <c r="O86" s="5"/>
     </row>
     <row r="87" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O87" s="1"/>
+      <c r="O87" s="5"/>
     </row>
     <row r="88" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O88" s="1"/>
+      <c r="O88" s="5"/>
     </row>
     <row r="89" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O89" s="1"/>
+      <c r="O89" s="5"/>
     </row>
     <row r="90" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O90" s="1"/>
+      <c r="O90" s="5"/>
     </row>
     <row r="91" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O91" s="1"/>
+      <c r="O91" s="5"/>
     </row>
     <row r="92" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O92" s="1"/>
+      <c r="O92" s="5"/>
     </row>
     <row r="93" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O93" s="1"/>
+      <c r="O93" s="5"/>
     </row>
     <row r="94" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O94" s="1"/>
+      <c r="O94" s="5"/>
     </row>
     <row r="95" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O95" s="1"/>
+      <c r="O95" s="5"/>
     </row>
     <row r="96" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O96" s="1"/>
+      <c r="O96" s="5"/>
     </row>
     <row r="97" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O97" s="1"/>
+      <c r="O97" s="5"/>
     </row>
     <row r="98" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O98" s="1"/>
+      <c r="O98" s="5"/>
     </row>
     <row r="99" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O99" s="1"/>
+      <c r="O99" s="5"/>
     </row>
     <row r="100" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O100" s="1"/>
+      <c r="O100" s="5"/>
     </row>
     <row r="101" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O101" s="1"/>
+      <c r="O101" s="5"/>
     </row>
     <row r="102" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O102" s="1"/>
+      <c r="O102" s="5"/>
     </row>
     <row r="103" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O103" s="1"/>
+      <c r="O103" s="5"/>
     </row>
     <row r="104" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O104" s="1"/>
+      <c r="O104" s="5"/>
     </row>
     <row r="105" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O105" s="1"/>
+      <c r="O105" s="5"/>
     </row>
     <row r="106" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O106" s="1"/>
+      <c r="O106" s="5"/>
     </row>
     <row r="107" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O107" s="1"/>
+      <c r="O107" s="5"/>
     </row>
     <row r="108" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O108" s="1"/>
+      <c r="O108" s="5"/>
     </row>
     <row r="109" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O109" s="1"/>
+      <c r="O109" s="5"/>
     </row>
     <row r="110" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O110" s="1"/>
+      <c r="O110" s="5"/>
     </row>
     <row r="111" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O111" s="1"/>
+      <c r="O111" s="5"/>
     </row>
     <row r="112" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O112" s="1"/>
+      <c r="O112" s="5"/>
     </row>
     <row r="113" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O113" s="1"/>
+      <c r="O113" s="5"/>
     </row>
     <row r="114" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O114" s="1"/>
+      <c r="O114" s="5"/>
     </row>
     <row r="115" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O115" s="1"/>
+      <c r="O115" s="5"/>
     </row>
     <row r="116" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O116" s="1"/>
+      <c r="O116" s="5"/>
     </row>
     <row r="117" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O117" s="1"/>
+      <c r="O117" s="5"/>
     </row>
     <row r="118" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O118" s="1"/>
+      <c r="O118" s="5"/>
     </row>
     <row r="119" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O119" s="1"/>
+      <c r="O119" s="5"/>
     </row>
     <row r="120" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O120" s="1"/>
+      <c r="O120" s="5"/>
     </row>
     <row r="121" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O121" s="1"/>
+      <c r="O121" s="5"/>
     </row>
     <row r="122" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O122" s="1"/>
+      <c r="O122" s="5"/>
     </row>
     <row r="123" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O123" s="1"/>
+      <c r="O123" s="5"/>
     </row>
     <row r="124" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O124" s="1"/>
+      <c r="O124" s="5"/>
     </row>
     <row r="125" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O125" s="1"/>
+      <c r="O125" s="5"/>
     </row>
     <row r="126" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O126" s="1"/>
+      <c r="O126" s="5"/>
     </row>
     <row r="127" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O127" s="1"/>
+      <c r="O127" s="5"/>
     </row>
     <row r="128" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O128" s="1"/>
+      <c r="O128" s="5"/>
     </row>
     <row r="129" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O129" s="1"/>
+      <c r="O129" s="5"/>
     </row>
     <row r="130" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O130" s="1"/>
+      <c r="O130" s="5"/>
     </row>
     <row r="131" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O131" s="1"/>
+      <c r="O131" s="5"/>
     </row>
     <row r="132" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O132" s="1"/>
+      <c r="O132" s="5"/>
     </row>
     <row r="133" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O133" s="1"/>
+      <c r="O133" s="5"/>
     </row>
     <row r="134" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O134" s="1"/>
+      <c r="O134" s="5"/>
     </row>
     <row r="135" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O135" s="1"/>
+      <c r="O135" s="5"/>
     </row>
     <row r="136" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O136" s="1"/>
+      <c r="O136" s="5"/>
     </row>
     <row r="137" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O137" s="1"/>
+      <c r="O137" s="5"/>
     </row>
     <row r="138" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O138" s="1"/>
+      <c r="O138" s="5"/>
     </row>
     <row r="139" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O139" s="1"/>
+      <c r="O139" s="5"/>
     </row>
     <row r="140" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O140" s="1"/>
+      <c r="O140" s="5"/>
     </row>
     <row r="141" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O141" s="1"/>
+      <c r="O141" s="5"/>
     </row>
     <row r="142" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O142" s="1"/>
+      <c r="O142" s="5"/>
     </row>
     <row r="143" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O143" s="1"/>
+      <c r="O143" s="5"/>
     </row>
     <row r="144" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O144" s="1"/>
+      <c r="O144" s="5"/>
     </row>
     <row r="145" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O145" s="1"/>
+      <c r="O145" s="5"/>
     </row>
     <row r="146" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O146" s="1"/>
+      <c r="O146" s="5"/>
     </row>
     <row r="147" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O147" s="1"/>
+      <c r="O147" s="5"/>
     </row>
     <row r="148" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O148" s="1"/>
+      <c r="O148" s="5"/>
     </row>
     <row r="149" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O149" s="1"/>
+      <c r="O149" s="5"/>
     </row>
     <row r="150" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O150" s="1"/>
+      <c r="O150" s="5"/>
     </row>
     <row r="151" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O151" s="1"/>
+      <c r="O151" s="5"/>
     </row>
     <row r="152" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O152" s="1"/>
+      <c r="O152" s="5"/>
     </row>
     <row r="153" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O153" s="1"/>
+      <c r="O153" s="5"/>
     </row>
     <row r="154" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O154" s="1"/>
+      <c r="O154" s="5"/>
     </row>
     <row r="155" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O155" s="1"/>
+      <c r="O155" s="5"/>
     </row>
     <row r="156" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O156" s="1"/>
+      <c r="O156" s="5"/>
     </row>
     <row r="157" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O157" s="1"/>
+      <c r="O157" s="5"/>
     </row>
     <row r="158" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O158" s="1"/>
+      <c r="O158" s="5"/>
     </row>
     <row r="159" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O159" s="1"/>
+      <c r="O159" s="5"/>
     </row>
     <row r="160" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O160" s="1"/>
+      <c r="O160" s="5"/>
     </row>
     <row r="161" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O161" s="1"/>
+      <c r="O161" s="5"/>
     </row>
     <row r="162" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O162" s="1"/>
+      <c r="O162" s="5"/>
     </row>
     <row r="163" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O163" s="1"/>
+      <c r="O163" s="5"/>
     </row>
     <row r="164" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O164" s="1"/>
+      <c r="O164" s="5"/>
     </row>
     <row r="165" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O165" s="1"/>
+      <c r="O165" s="5"/>
     </row>
     <row r="166" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O166" s="1"/>
+      <c r="O166" s="5"/>
     </row>
     <row r="167" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O167" s="1"/>
+      <c r="O167" s="5"/>
     </row>
     <row r="168" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O168" s="1"/>
+      <c r="O168" s="5"/>
     </row>
     <row r="169" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O169" s="1"/>
+      <c r="O169" s="5"/>
     </row>
     <row r="170" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O170" s="1"/>
+      <c r="O170" s="5"/>
     </row>
     <row r="171" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O171" s="1"/>
+      <c r="O171" s="5"/>
     </row>
     <row r="172" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O172" s="1"/>
+      <c r="O172" s="5"/>
     </row>
     <row r="173" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O173" s="1"/>
+      <c r="O173" s="5"/>
     </row>
     <row r="174" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O174" s="1"/>
+      <c r="O174" s="5"/>
     </row>
     <row r="175" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O175" s="1"/>
+      <c r="O175" s="5"/>
     </row>
     <row r="176" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O176" s="1"/>
+      <c r="O176" s="5"/>
     </row>
     <row r="177" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O177" s="1"/>
+      <c r="O177" s="5"/>
     </row>
     <row r="178" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O178" s="1"/>
+      <c r="O178" s="5"/>
     </row>
     <row r="179" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O179" s="1"/>
+      <c r="O179" s="5"/>
     </row>
     <row r="180" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O180" s="1"/>
+      <c r="O180" s="5"/>
     </row>
     <row r="181" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O181" s="1"/>
+      <c r="O181" s="5"/>
     </row>
     <row r="182" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O182" s="1"/>
+      <c r="O182" s="5"/>
     </row>
     <row r="183" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O183" s="1"/>
+      <c r="O183" s="5"/>
     </row>
     <row r="184" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O184" s="1"/>
+      <c r="O184" s="5"/>
     </row>
     <row r="185" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O185" s="1"/>
+      <c r="O185" s="5"/>
     </row>
     <row r="186" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O186" s="1"/>
+      <c r="O186" s="5"/>
     </row>
     <row r="187" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O187" s="1"/>
+      <c r="O187" s="5"/>
     </row>
     <row r="188" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O188" s="1"/>
+      <c r="O188" s="5"/>
     </row>
     <row r="189" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O189" s="1"/>
+      <c r="O189" s="5"/>
     </row>
     <row r="190" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O190" s="1"/>
+      <c r="O190" s="5"/>
     </row>
     <row r="191" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O191" s="1"/>
+      <c r="O191" s="5"/>
     </row>
     <row r="192" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O192" s="1"/>
+      <c r="O192" s="5"/>
     </row>
     <row r="193" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O193" s="1"/>
+      <c r="O193" s="5"/>
     </row>
     <row r="194" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O194" s="1"/>
+      <c r="O194" s="5"/>
     </row>
     <row r="195" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O195" s="1"/>
+      <c r="O195" s="5"/>
     </row>
     <row r="196" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O196" s="1"/>
+      <c r="O196" s="5"/>
     </row>
     <row r="197" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O197" s="1"/>
+      <c r="O197" s="5"/>
     </row>
     <row r="198" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O198" s="1"/>
+      <c r="O198" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1585,7 +1650,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" style="13"/>
+    <col min="1" max="1" width="11.19921875" style="7"/>
     <col min="2" max="2" width="19.796875" customWidth="1"/>
     <col min="3" max="3" width="20.3984375" customWidth="1"/>
     <col min="4" max="6" width="23.09765625" customWidth="1"/>
@@ -1599,68 +1664,68 @@
     <col min="20" max="20" width="16.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="7" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B2" t="s">
@@ -1678,10 +1743,10 @@
       <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>50</v>
       </c>
       <c r="I2" t="s">
@@ -1711,7 +1776,7 @@
       <c r="Q2" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="5" t="s">
         <v>56</v>
       </c>
       <c r="S2" t="s">
@@ -1722,69 +1787,69 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="5" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>